<commit_message>
Atualização no dia da entrega do artigo
</commit_message>
<xml_diff>
--- a/Estatistica_lstm_teste.xlsx
+++ b/Estatistica_lstm_teste.xlsx
@@ -253,13 +253,13 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B7"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -275,7 +275,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>0.0269128957991327</v>
+        <v>0.0230276641589093</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -283,7 +283,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>0.0220899071518288</v>
+        <v>0.0202303338201754</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -291,7 +291,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>1.18182369356661E-005</v>
+        <v>6.34954274860123E-005</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -299,7 +299,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>0.135829849037817</v>
+        <v>0.11609268046095</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -307,7 +307,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>0.021221672236186</v>
+        <v>0.0175501124960426</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -315,7 +315,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>0.0056094345685541</v>
+        <v>0.0158290896823424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>